<commit_message>
fixed the 'name not being scraped' issue
</commit_message>
<xml_diff>
--- a/google_maps_data.xlsx
+++ b/google_maps_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -458,44 +458,44 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Temple Dental</t>
+          <t>The Welbeck Clinic</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Fleet Street Clinic, 29 Fleet St, Temple, London EC4Y 1AA, Royaume-Uni</t>
+          <t>20 Welbeck St, London W1G 8ED, Royaume-Uni</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>templedental.com</t>
+          <t>thewelbeckclinic.co.uk</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>+44 20 8175 8892</t>
+          <t>+44 20 7486 8100</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>The Welbeck Clinic - Cosmetic Dentist</t>
+          <t>French Dentist London</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>20 Welbeck St, London W1G 8ED, Royaume-Uni</t>
+          <t>71 Queen's Gate, South Kensington, London SW7 5JT, Royaume-Uni</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>thewelbeckclinic.co.uk</t>
+          <t>drsadone.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>+44 20 7486 8100</t>
+          <t>+44 20 7373 6899</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
v2: added reviews scraping + scrolling
</commit_message>
<xml_diff>
--- a/google_maps_data.xlsx
+++ b/google_maps_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,115 +454,175 @@
           <t>phone_number</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>reviews_count</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>reviews_average</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>The Welbeck Clinic</t>
+          <t>Dr Pascal MARIN</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>20 Welbeck St, London W1G 8ED, Royaume-Uni</t>
+          <t>5 Rue Crétet, 75009 Paris, France</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>thewelbeckclinic.co.uk</t>
+          <t>doctolib.fr</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>+44 20 7486 8100</t>
-        </is>
+          <t>+33 6 75 15 49 16</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3.4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>French Dentist London</t>
+          <t>Dr. Charlotte Parment</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>71 Queen's Gate, South Kensington, London SW7 5JT, Royaume-Uni</t>
+          <t>cabinet médical ipso Saint Martin, 323 Rue Saint-Martin, 75003 Paris, France</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>drsadone.com</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>+44 20 7373 6899</t>
-        </is>
+          <t>ipso.paris</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>London Dental Centre</t>
+          <t>Dr Claire Paris</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>109 Lever St, London EC1V 3RQ, Royaume-Uni</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>thelondondentalcentre.co.uk</t>
-        </is>
-      </c>
+          <t>86 Rue de l'Université, 75007 Paris, France</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>+44 20 7608 0806</t>
-        </is>
+          <t>+33 1 40 62 95 28</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Dental Smiles London Chalton Street</t>
+          <t>Dr Nancy Salzman</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>30-32 Chalton St, London NW1 1JB, Royaume-Uni</t>
+          <t>1 Av. de Lowendal, 75007 Paris, France</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dentalsmileslondon.co.uk</t>
+          <t>doctor-salzman.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>+44 20 3757 5272</t>
-        </is>
+          <t>+33 1 45 63 18 43</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>35</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4.8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Pall Mall Dental London</t>
+          <t>Docteur Franck Besse</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>15 Pall Mall, St. James's, London SW1Y 5LU, Royaume-Uni</t>
+          <t>45 Rue de Lancry, 75010 Paris, France</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>pallmalldental.co.uk</t>
+          <t>doctolib.fr</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>+44 20 7766 7150</t>
-        </is>
+          <t>+33 1 44 85 26 83</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>24</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Docteur Simon OHAYON- English speaking doctor- International medical center</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>48 BIS Rue des Belles Feuilles, 75116 Paris, France</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>doctolib.fr</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>+33 6 58 80 18 38</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>94</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed infinit scrolling bug
</commit_message>
<xml_diff>
--- a/google_maps_data.xlsx
+++ b/google_maps_data.xlsx
@@ -468,161 +468,169 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Dr Pascal MARIN</t>
+          <t>ELSAN</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5 Rue Crétet, 75009 Paris, France</t>
+          <t>58 bis Rue La Boétie, 75008 Paris, France</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>doctolib.fr</t>
+          <t>elsan.care</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>+33 6 75 15 49 16</t>
+          <t>+33 1 58 56 16 80</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="F2" t="n">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dr. Charlotte Parment</t>
+          <t>Dentego</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>cabinet médical ipso Saint Martin, 323 Rue Saint-Martin, 75003 Paris, France</t>
+          <t>19 Rue de Passy, 75016 Paris, France</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ipso.paris</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
+          <t>dentego.fr</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>+33 1 88 88 09 09</t>
+        </is>
+      </c>
       <c r="E3" t="n">
+        <v>104</v>
+      </c>
+      <c r="F3" t="n">
         <v>4</v>
-      </c>
-      <c r="F3" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dr Claire Paris</t>
+          <t>Paris Dental Studios - MARAIS</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>86 Rue de l'Université, 75007 Paris, France</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
+          <t>28 Rue Meslay, 75003 Paris, France</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>parisdentalstudios.com</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>+33 1 40 62 95 28</t>
+          <t>+33 9 52 34 01 45</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>204</v>
       </c>
       <c r="F4" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Dr Nancy Salzman</t>
+          <t>Clinadent - Centre dentaire Paris 16 Victor Hugo</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1 Av. de Lowendal, 75007 Paris, France</t>
+          <t>3 Pl. Victor Hugo, 75016 Paris, France</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>doctor-salzman.com</t>
+          <t>centre-dentaire-paris16.fr</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>+33 1 45 63 18 43</t>
+          <t>+33 1 42 25 40 79</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>35</v>
+        <v>601</v>
       </c>
       <c r="F5" t="n">
-        <v>4.8</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Docteur Franck Besse</t>
+          <t>Dentego</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>45 Rue de Lancry, 75010 Paris, France</t>
+          <t>111 Av. du Général Leclerc, 75014 Paris, France</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>doctolib.fr</t>
+          <t>dentego.fr</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>+33 1 44 85 26 83</t>
+          <t>+33 1 40 43 41 00</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>24</v>
+        <v>307</v>
       </c>
       <c r="F6" t="n">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Docteur Simon OHAYON- English speaking doctor- International medical center</t>
+          <t>Place dentaire - Centre dentaire Paris Nation Saint Antoine</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>48 BIS Rue des Belles Feuilles, 75116 Paris, France</t>
+          <t>238 bis Rue du Faubourg Saint-Antoine, 75012 Paris, France</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>doctolib.fr</t>
+          <t>centre-dentaire-nation-saint-antoine.fr</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>+33 6 58 80 18 38</t>
+          <t>+33 1 42 55 55 42</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F7" t="n">
-        <v>4.1</v>
+        <v>3.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added example data with latitude and longitude
</commit_message>
<xml_diff>
--- a/google_maps_data.xlsx
+++ b/google_maps_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,557 +464,853 @@
           <t>reviews_average</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>latitude</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>longitude</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Enabling Projects (London Planning Consultancy)</t>
+          <t>Restaurant Y Panaderia Latina</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>40 Sandringham Rd, London NW11 9DP, Royaume-Uni</t>
+          <t>3221 W Davis St, Dallas, TX 75211, États-Unis</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>enablinguk.com</t>
+          <t>latinarestaurante.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>+44 20 8381 4311</t>
+          <t>+1 214-337-4470</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>356</v>
       </c>
       <c r="F2" t="n">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>32.7498452</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-97.1703813</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Budget Photographer London</t>
+          <t>Sabor Latino</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>37 Kirkham St, London SE18 2JS, Royaume-Uni</t>
+          <t>5431 E Grand Ave, Dallas, TX 75223, États-Unis</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>budgetphotographerlondon.co.uk</t>
+          <t>saborlatinodallas.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>+44 7769 313560</t>
+          <t>+1 817-243-5500</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>120</v>
+        <v>174</v>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>4.3</v>
+      </c>
+      <c r="G3" t="n">
+        <v>32.7498452</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-97.1703813</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Karolina Heller Photography</t>
+          <t>Miriam Cocina Latina</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>32 Davies St, London W1K 4ND, Royaume-Uni</t>
+          <t>2015 Woodall Rodgers Fwy, Dallas, TX 75201, États-Unis</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>karolinaheller.co.uk</t>
+          <t>miriamcocina.com</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>+44 7522 011306</t>
+          <t>+1 214-855-5275</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>100</v>
+        <v>910</v>
       </c>
       <c r="F4" t="n">
-        <v>5</v>
+        <v>4.6</v>
+      </c>
+      <c r="G4" t="n">
+        <v>32.7498452</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-97.1703813</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Events Photographer London</t>
+          <t>Zaguan Latin Café &amp; Bakery</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>58 Fitzroy St, London W1T 5BU, Royaume-Uni</t>
+          <t>Zaguan Latin Cafe &amp; Bakery, 2604 Oak Lawn Ave, Dallas, TX 75219, États-Unis</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>freelanceeventsphotographer.co.uk</t>
+          <t>zaguan.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>+44 20 3951 7175</t>
+          <t>+1 214-219-8393</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>164</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>5</v>
+        <v>4.1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>32.7498452</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-97.1703813</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Photographerforhire.co.uk</t>
+          <t>Gloria's Latin Cuisine</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5 Torrens St, London EC1V 1NQ, Royaume-Uni</t>
+          <t>3715 Greenville Ave, Dallas, TX 75206, États-Unis</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>photographerforhire.co.uk</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
+          <t>gloriascuisine.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>+1 214-874-0088</t>
+        </is>
+      </c>
       <c r="E6" t="n">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>5</v>
+        <v>4.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>32.7498452</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-97.1703813</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Douglas Fry Wedding Photographer London</t>
+          <t>Gloria's Latin Cuisine</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>11 Regency Terrace, South Kensington, London SW7 3QW, Royaume-Uni</t>
+          <t>600 N Bishop Ave, Dallas, TX 75208, États-Unis</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>douglasfry.com</t>
+          <t>gloriascuisine.com</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>+44 20 7193 9414</t>
+          <t>+1 214-948-3672</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
-        <v>5</v>
+        <v>4.4</v>
+      </c>
+      <c r="G7" t="n">
+        <v>32.7498452</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-97.1703813</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Corporate Photographer</t>
+          <t>Tienda &amp; Restaurant Latina</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>22 Wenlock Rd, London N1 7GU, Royaume-Uni</t>
+          <t>4950 W Illinois Ave #115, Dallas, TX 75211, États-Unis</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>charlessturge.com</t>
+          <t>latinarestaurante.com</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>+44 20 7737 5509</t>
+          <t>+1 214-330-0011</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>49</v>
+        <v>272</v>
       </c>
       <c r="F8" t="n">
-        <v>4.9</v>
+        <v>3.8</v>
+      </c>
+      <c r="G8" t="n">
+        <v>32.7498452</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-97.1703813</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IvanWeiss.London Headshot Photography</t>
+          <t>Wild Salsa</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3, The Old School, 146 York Wy, London N1 0AE, Royaume-Uni</t>
+          <t>1800 Main St, Dallas, TX 75201, États-Unis</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ivanweiss.london</t>
+          <t>wildsalsarestaurant.com</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>+44 7528 726626</t>
+          <t>+1 214-741-9453</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>240</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>5</v>
+        <v>4.4</v>
+      </c>
+      <c r="G9" t="n">
+        <v>32.7498452</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-97.1703813</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Emma-Jane Photography</t>
+          <t>Restaurant Latino</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1st Floor, 85 Great Portland St, London W1W 7LT, Royaume-Uni</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>emma-janephotography.co.uk</t>
-        </is>
-      </c>
+          <t>14500 S Josey Ln #101, Dallas, TX 75234, États-Unis</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>+44 7913 743677</t>
+          <t>+1 972-620-4954</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>84</v>
+        <v>172</v>
       </c>
       <c r="F10" t="n">
-        <v>5</v>
+        <v>3.8</v>
+      </c>
+      <c r="G10" t="n">
+        <v>32.9443412</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-97.1783298</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Serena Bolton Photography</t>
+          <t>Cafe Salsera</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>144 Iffley Rd, London W6 0PE, Royaume-Uni</t>
+          <t>2610 Elm St, Dallas, TX 75226, États-Unis</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>serenabolton.com</t>
+          <t>cafesalsera.com</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>+44 7958 511819</t>
+          <t>+1 469-518-1500</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>171</v>
+        <v>682</v>
       </c>
       <c r="F11" t="n">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="G11" t="n">
+        <v>32.9443412</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-97.1783298</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>London Portrait Photographer</t>
+          <t>El Bolero Cocina Mexicana</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>149 Crofton Park Rd, London SE4 1AJ, Royaume-Uni</t>
+          <t>1201 Oak Lawn Ave #160, Dallas, TX 75207, États-Unis</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>davidwoolfall.com</t>
+          <t>elboleromexican.com</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>+44 7802 819308</t>
+          <t>+1 214-741-1986</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>5</v>
+        <v>4.1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>32.9443412</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-97.1783298</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>WeShootYou | Family Photographer London</t>
+          <t>Salsa Limón</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>99, Nuriad House, Bow, London E3 5GQ, Royaume-Uni</t>
+          <t>411 N Akard St, Dallas, TX 75201, États-Unis</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>weshootyou.co.uk</t>
+          <t>salsalimon.com</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>+44 7724 098255</t>
+          <t>+1 972-803-4388</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>5</v>
+        <v>4.5</v>
+      </c>
+      <c r="G13" t="n">
+        <v>32.9443412</v>
+      </c>
+      <c r="H13" t="n">
+        <v>-97.1783298</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Dan Burman Photography</t>
+          <t>Havana Cafe-Mojito Bar</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>14 Bacon St, London E1 6LF, Royaume-Uni</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>londonphotographer.co.uk</t>
-        </is>
-      </c>
+          <t>1152 N Buckner Blvd #126, Dallas, TX 75218, États-Unis</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>+44 20 7193 7633</t>
+          <t>+1 214-660-9611</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>5</v>
+        <v>4.4</v>
+      </c>
+      <c r="G14" t="n">
+        <v>32.8342759</v>
+      </c>
+      <c r="H14" t="n">
+        <v>-96.9905284</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Hadi Photography London</t>
+          <t>Cafe Madrid</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>9 Hammersmith Rd, London W14 8XJ, Royaume-Uni</t>
+          <t>4501 Travis St, Dallas, TX 75205, États-Unis</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>hadiphotographylondon.com</t>
+          <t>cafemadrid-dallas.com</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>+44 7444 946465</t>
+          <t>+1 214-528-1731</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>81</v>
+        <v>927</v>
       </c>
       <c r="F15" t="n">
-        <v>5</v>
+        <v>4.4</v>
+      </c>
+      <c r="G15" t="n">
+        <v>32.8342759</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-96.9905284</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Simon Callaghan Commercial Photography London</t>
+          <t>Gloria's Latin Cuisine</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>39 Choumert Sq, London SE15 4RE, Royaume-Uni</t>
+          <t>3223 Lemmon Ave, Dallas, TX 75204, États-Unis</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>simoncallaghanphotography.com</t>
+          <t>gloriascuisine.com</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>+44 7736 072373</t>
+          <t>+1 214-303-1166</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>5</v>
+        <v>4.4</v>
+      </c>
+      <c r="G16" t="n">
+        <v>32.8342759</v>
+      </c>
+      <c r="H16" t="n">
+        <v>-96.9905284</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Headshot London</t>
+          <t>Gloria's Latin Cuisine</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>107 Clifton St, London EC2A 4LG, Royaume-Uni</t>
+          <t>4140 Lemmon Ave, Dallas, TX 75219, États-Unis</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>headshotlondon.co.uk</t>
+          <t>gloriascuisine.com</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>+44 20 3289 9054</t>
+          <t>+1 214-521-7576</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>22</v>
+        <v>849</v>
       </c>
       <c r="F17" t="n">
-        <v>4.8</v>
+        <v>4.4</v>
+      </c>
+      <c r="G17" t="n">
+        <v>32.8342759</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-96.9905284</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Andrew Mason Photography</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
+          <t>Las Palmas Restaurant</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3957 Belt Line Rd, Addison, TX 75001, États-Unis</t>
+        </is>
+      </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>andrew-mason.com</t>
+          <t>laspalmasrestaurante.com</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>+44 7779 082909</t>
+          <t>+1 469-665-8958</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>4.9</v>
+        <v>4.1</v>
+      </c>
+      <c r="G18" t="n">
+        <v>32.9539978</v>
+      </c>
+      <c r="H18" t="n">
+        <v>-97.1360389</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Old &amp; New Photography Studio</t>
+          <t>Beto &amp; Son</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>156 Brompton Rd, London SW3 1HW, Royaume-Uni</t>
+          <t>3011 Gulden Ln #108, Dallas, TX 75212, États-Unis</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>oldnewstudio.com</t>
+          <t>betoandsondallas.com</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>+44 7423 330541</t>
+          <t>+1 469-249-8590</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>518</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
-        <v>4.9</v>
+        <v>4.3</v>
+      </c>
+      <c r="G19" t="n">
+        <v>32.9539978</v>
+      </c>
+      <c r="H19" t="n">
+        <v>-97.1360389</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>The Snapper - London wedding photographer</t>
+          <t>Ocho Latin Cuisine Events</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Porden Rd, Brixton Hill, London SW2 5RT, Royaume-Uni</t>
+          <t>369 Jefferson Blvd, Dallas, TX 75208, États-Unis</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>the-snapper.com</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>+44 7780 994204</t>
-        </is>
-      </c>
+          <t>ochooc.com</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
-        <v>187</v>
+        <v>134</v>
       </c>
       <c r="F20" t="n">
-        <v>5</v>
+        <v>4.1</v>
+      </c>
+      <c r="G20" t="n">
+        <v>32.7433967</v>
+      </c>
+      <c r="H20" t="n">
+        <v>-97.11642449999999</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Splento</t>
+          <t>Meso Maya Comida y Copas</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>House, 92 Albert Embankment Tintagel, London SE1 7TY, Royaume-Uni</t>
+          <t>1611 McKinney Ave, Dallas, TX 75202, États-Unis</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>splento.com</t>
+          <t>mesomaya.com</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>+44 20 8123 1838</t>
+          <t>+1 214-484-6555</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
-        <v>4.8</v>
+        <v>4.5</v>
+      </c>
+      <c r="G21" t="n">
+        <v>32.7433967</v>
+      </c>
+      <c r="H21" t="n">
+        <v>-97.11642449999999</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Campuzano Mexican Food</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2618 Oak Lawn Ave, Dallas, TX 75219, États-Unis</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>campuzanomexicanfood.com</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>+1 214-526-0100</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="G22" t="n">
+        <v>32.7433967</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-97.11642449999999</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>La Duni Latin Cafe</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2612 Irving Blvd, Dallas, TX 75207, États-Unis</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ladunihub.com</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>+1 214-520-7300</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>859</v>
+      </c>
+      <c r="F23" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="G23" t="n">
+        <v>32.7433967</v>
+      </c>
+      <c r="H23" t="n">
+        <v>-97.11642449999999</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Mi Sazon Mexican Restaurant</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>3505 S Polk St, Dallas, TX 75224, États-Unis</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>misazonrestaurant.com</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>+1 214-375-3333</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>745</v>
+      </c>
+      <c r="F24" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="G24" t="n">
+        <v>32.7433967</v>
+      </c>
+      <c r="H24" t="n">
+        <v>-97.11642449999999</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Si Tapas</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2207 Allen St, Dallas, TX 75204, États-Unis</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>sitapasdallas.com</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>+1 214-720-0324</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>980</v>
+      </c>
+      <c r="F25" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="G25" t="n">
+        <v>32.7433967</v>
+      </c>
+      <c r="H25" t="n">
+        <v>-97.11642449999999</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Te Deseo</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2700 Olive St, Dallas, TX 75201, États-Unis</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>tedeseo.com</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>+1 214-646-1314</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="G26" t="n">
+        <v>32.7433967</v>
+      </c>
+      <c r="H26" t="n">
+        <v>-97.11642449999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>